<commit_message>
update đề thi 1
</commit_message>
<xml_diff>
--- a/final-test/de-so-1/mau-excel-de-so-1.xlsx
+++ b/final-test/de-so-1/mau-excel-de-so-1.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nentang\dao-tao\fpt\Tin-hoc\src\learning.nentang.vn-tin-hoc-can-ban\final-test\de-so-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DE7207-C644-4C21-8F02-BEFF6B6A0BE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250AA96E-55A4-46C2-8DB9-8BF7F1D25718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7860" yWindow="3795" windowWidth="18030" windowHeight="13410" xr2:uid="{047F9B6D-7720-4871-B4EF-51007955FAFB}"/>
+    <workbookView xWindow="540" yWindow="6900" windowWidth="18030" windowHeight="13410" xr2:uid="{047F9B6D-7720-4871-B4EF-51007955FAFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
   <si>
     <t>BẢNG CHI TIẾT THÔNG TIN KHÁCH HÀNG CỦA 1 KHÁCH SẠN</t>
   </si>
@@ -186,6 +186,211 @@
   </si>
   <si>
     <t>Tổng thành tiền</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Câu 1 (1đ): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>tính cột Tuổi của Khách hàng, biết rằng:</t>
+    </r>
+  </si>
+  <si>
+    <t>Tuổi = năm hiện tại – năm sinh</t>
+  </si>
+  <si>
+    <t>Lưu ý: sử dụng hàm NOW và hàm YEAR để thực hiện.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Câu 2 (1đ): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>tính cột Tiền ăn, biết rằng:</t>
+    </r>
+  </si>
+  <si>
+    <t>Tiền ăn = tổng số ngày ở * đơn giá khẩu phần ăn</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2 ký tự cuối của cột Mã số là Mã khẩu phần ăn, bảng dò Khẩu phần ăn là </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Bảng 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Lưu ý: sử dụng hàm HLOOPUP để thực hiện.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Câu 3 (1.5đ): </t>
+  </si>
+  <si>
+    <r>
+      <t>Câu 3a:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Tính cột Thành tiền tuần, biết rằng:</t>
+    </r>
+  </si>
+  <si>
+    <t>Thành tiền tuần = số tuần ở * đơn giá tuần theo loại phòng</t>
+  </si>
+  <si>
+    <t>Số tuần ở = Tổng số ngày ở / 7 (lấy số nguyên)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3 ký tự đầu của cột Mã số là Mã loại phòng, bảng dò Đơn giá tuần là </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Bảng 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Câu 3b:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Tính cột Thành tiền ngày, biết rằng:</t>
+    </r>
+  </si>
+  <si>
+    <t>Thành tiền ngày = số ngày ở * đơn giá ngày theo loại phòng</t>
+  </si>
+  <si>
+    <t>Số ngày ở = Tổng số ngày ở % 7 (chia lấy dư)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3 ký tự đầu của cột Mã số là Mã loại phòng, bảng dò Đơn giá ngày là </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Bảng 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Lưu ý: sử dụng hàm VLOOKUP để thực hiện.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Câu 4 (0.5đ): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>tính cột Tổng cộng, biết rằng:</t>
+    </r>
+  </si>
+  <si>
+    <t>Tổng cộng = Thành tiền tuần + Thành tiền ngày</t>
+  </si>
+  <si>
+    <t>Tổng thành tiền = SUM(cột Tổng cộng)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Câu 5 (1đ): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">tính cột thống kê doanh thu (cột Tổng cộng) theo từng loại phòng trong </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Bảng 4.</t>
+    </r>
+  </si>
+  <si>
+    <t>Lưu ý: sử dụng hàm SUMIFS để thống kê.</t>
   </si>
 </sst>
 </file>
@@ -194,9 +399,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -234,6 +439,13 @@
     <font>
       <sz val="13"/>
       <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="13"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -347,17 +559,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -367,22 +591,18 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="5" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="168" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -703,10 +923,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65EBFDE9-DE08-438F-BE37-9F7612A72CB0}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -726,454 +946,586 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" s="14" customFormat="1" ht="33" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+    </row>
+    <row r="2" spans="1:11" s="8" customFormat="1" ht="33" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>36322</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>44625</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>44636</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>35100</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>44626</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>44640</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>35338</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>44630</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>44650</v>
       </c>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>34196</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>44643</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>44652</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>35998</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>44637</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>44681</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>27495</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>44642</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>44647</v>
       </c>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>31278</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>44650</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>44672</v>
       </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>35627</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>44654</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>44672</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>33984</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>44656</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>44693</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>33251</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>44663</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>44678</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="J13" s="17" t="s">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="J13" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="K13" s="16"/>
+      <c r="K13" s="10"/>
     </row>
     <row r="16" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="E16" s="6" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="E16" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="8"/>
-      <c r="J16" s="6" t="s">
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="16"/>
+      <c r="J16" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="K16" s="8"/>
+      <c r="K16" s="16"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="K17" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="12">
         <v>260000</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="12">
         <v>45000</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="12">
         <v>20000</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="12">
         <v>30000</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="12">
         <v>50000</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="11"/>
+      <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B19" s="12">
         <v>250000</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="12">
         <v>40000</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="J19" s="4" t="s">
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="J19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K19" s="11"/>
+      <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B20" s="12">
         <v>210000</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="12">
         <v>36000</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K20" s="11"/>
+      <c r="K20" s="6"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="12">
         <v>190000</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="12">
         <v>30000</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="K21" s="11"/>
+      <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="J22" s="12" t="s">
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="J22" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="K22" s="12"/>
+      <c r="K22" s="17"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27"/>
+      <c r="B27" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44"/>
+      <c r="B44" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45"/>
+      <c r="B45" s="19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1187,5 +1539,6 @@
     <mergeCell ref="A13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>